<commit_message>
Improve test file for detecting DateTime type cell.
The test files checked only subset of predefined formats (only 14 and 22). The predefined formats 15 (d-mmm-yy) and 16 (d-mmm) were added to the test files.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/TryToLoad/CellsWithDateTimeDataTypeOrFormatting.xlsx
+++ b/ClosedXML.Tests/Resource/TryToLoad/CellsWithDateTimeDataTypeOrFormatting.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="139" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3542AAF4-040F-4AA8-889F-6A40A0352651}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\TryToLoad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A277C063-9554-4C7A-A117-3E8CEDFBABBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Format</t>
   </si>
@@ -82,6 +87,12 @@
   </si>
   <si>
     <t>Date 14/03/2012 (UK)</t>
+  </si>
+  <si>
+    <t>Date 14-Mar</t>
+  </si>
+  <si>
+    <t>Date 14-Mar-12</t>
   </si>
 </sst>
 </file>
@@ -89,21 +100,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="13">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="171" formatCode="m/d;@"/>
-    <numFmt numFmtId="173" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="174" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="175" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="177" formatCode="[$-409]mmm\-yy;@"/>
-    <numFmt numFmtId="178" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="181" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="m/d;@"/>
+    <numFmt numFmtId="168" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="173" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="174" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="175" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,25 +158,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,20 +493,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -512,11 +525,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:C6" si="0">B2</f>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <f t="shared" ref="C2:C17" si="0">B2</f>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -528,7 +541,7 @@
         <v>40982.563138888887</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -540,7 +553,7 @@
         <v>40982.563138888887</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -552,7 +565,7 @@
         <v>40982.563138888887</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -564,7 +577,7 @@
         <v>40982.563138888887</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -572,11 +585,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C8" si="1">B7</f>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -584,11 +597,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="1"/>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -596,11 +609,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ref="C9:C10" si="2">B9</f>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -608,11 +621,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="2"/>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -620,11 +633,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" ref="C11:C12" si="3">B11</f>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
@@ -632,11 +645,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="3"/>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
@@ -644,11 +657,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C13:C14" si="4">B13</f>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -656,11 +669,11 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="4"/>
-        <v>40982.563138888887</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -668,7 +681,31 @@
         <v>40982.563138888887</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" ref="C15" si="5">B15</f>
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="19">
+        <v>40982.563138888887</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>40982.563138888887</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="18">
+        <v>40982.563138888887</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
         <v>40982.563138888887</v>
       </c>
     </row>

</xml_diff>